<commit_message>
menulist for db 설계서 -> typo
</commit_message>
<xml_diff>
--- a/doc/ONCE_DB설계서150705.xlsx
+++ b/doc/ONCE_DB설계서150705.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="580" windowWidth="18080" windowHeight="19020"/>
+    <workbookView xWindow="14940" yWindow="460" windowWidth="18080" windowHeight="19020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1349,9 +1349,6 @@
     <t>SUBTOTAL - DISCOUNT</t>
   </si>
   <si>
-    <t>SALE Table quntity 추가, RECEIPT subtotal discount 추가</t>
-  </si>
-  <si>
     <t>MENU_WHIP</t>
   </si>
   <si>
@@ -1368,13 +1365,16 @@
   </si>
   <si>
     <t>휘핑이 기본으로 들어가는경우 T else F</t>
+  </si>
+  <si>
+    <t>SALE Table quntity 추가, RECEIPT subtotal discount 추가, MENU WHIP 추가</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1438,11 +1438,6 @@
       <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Airal"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1772,14 +1767,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1787,22 +1776,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1819,7 +1795,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준 2" xfId="1"/>
@@ -2155,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2169,18 +2164,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="83" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -2201,15 +2196,15 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="77"/>
+      <c r="A2" s="84"/>
       <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
       <c r="F2" s="24" t="s">
         <v>2</v>
       </c>
@@ -2237,15 +2232,15 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="77"/>
+      <c r="A3" s="84"/>
       <c r="B3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
       <c r="F3" s="24" t="s">
         <v>5</v>
       </c>
@@ -2304,15 +2299,15 @@
       <c r="A5" s="65">
         <v>42190</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="90" t="s">
         <v>179</v>
       </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2333,18 +2328,18 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="44">
-        <v>2015.816</v>
-      </c>
-      <c r="B6" s="81" t="s">
-        <v>187</v>
-      </c>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
+      <c r="A6" s="65">
+        <v>42232</v>
+      </c>
+      <c r="B6" s="90" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -2420,16 +2415,16 @@
       <c r="B9" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="71" t="s">
+      <c r="D9" s="75"/>
+      <c r="E9" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2453,15 +2448,15 @@
       <c r="A10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -2485,15 +2480,15 @@
       <c r="A11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B11" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -2828,16 +2823,16 @@
       <c r="B21" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="72" t="s">
+      <c r="C21" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="69"/>
-      <c r="E21" s="71" t="s">
+      <c r="D21" s="75"/>
+      <c r="E21" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -2861,15 +2856,15 @@
       <c r="A22" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -2893,15 +2888,15 @@
       <c r="A23" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="70" t="s">
+      <c r="B23" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -3092,7 +3087,7 @@
       <c r="F28" s="30"/>
       <c r="G28" s="30"/>
       <c r="H28" s="47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -3128,7 +3123,7 @@
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
       <c r="H29" s="47" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -3151,10 +3146,10 @@
     </row>
     <row r="30" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="66" t="s">
+        <v>187</v>
+      </c>
+      <c r="B30" s="66" t="s">
         <v>188</v>
-      </c>
-      <c r="B30" s="66" t="s">
-        <v>189</v>
       </c>
       <c r="C30" s="43">
         <v>1</v>
@@ -3163,10 +3158,10 @@
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
       <c r="G30" s="61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H30" s="67" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -3370,16 +3365,16 @@
       <c r="B36" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="C36" s="72" t="s">
+      <c r="C36" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="69"/>
-      <c r="E36" s="71" t="s">
+      <c r="D36" s="75"/>
+      <c r="E36" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="69"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -3403,15 +3398,15 @@
       <c r="A37" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="69"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -3435,15 +3430,15 @@
       <c r="A38" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="68" t="s">
+      <c r="B38" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="69"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="75"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -3682,16 +3677,16 @@
       <c r="B45" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="73" t="s">
+      <c r="C45" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="74"/>
-      <c r="E45" s="75" t="s">
+      <c r="D45" s="72"/>
+      <c r="E45" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="F45" s="74"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="74"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="72"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
@@ -3715,15 +3710,15 @@
       <c r="A46" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="68" t="s">
+      <c r="B46" s="74" t="s">
         <v>152</v>
       </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="69"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="69"/>
+      <c r="C46" s="75"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="75"/>
+      <c r="F46" s="75"/>
+      <c r="G46" s="75"/>
+      <c r="H46" s="75"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -3747,15 +3742,15 @@
       <c r="A47" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="70" t="s">
+      <c r="B47" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="69"/>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="69"/>
-      <c r="G47" s="69"/>
-      <c r="H47" s="69"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="75"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
@@ -3984,16 +3979,16 @@
       <c r="B54" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="C54" s="72" t="s">
+      <c r="C54" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="69"/>
-      <c r="E54" s="71" t="s">
+      <c r="D54" s="75"/>
+      <c r="E54" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="F54" s="69"/>
-      <c r="G54" s="69"/>
-      <c r="H54" s="69"/>
+      <c r="F54" s="75"/>
+      <c r="G54" s="75"/>
+      <c r="H54" s="75"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -4017,15 +4012,15 @@
       <c r="A55" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="68" t="s">
+      <c r="B55" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="C55" s="69"/>
-      <c r="D55" s="69"/>
-      <c r="E55" s="69"/>
-      <c r="F55" s="69"/>
-      <c r="G55" s="69"/>
-      <c r="H55" s="69"/>
+      <c r="C55" s="75"/>
+      <c r="D55" s="75"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="75"/>
+      <c r="G55" s="75"/>
+      <c r="H55" s="75"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -4049,15 +4044,15 @@
       <c r="A56" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B56" s="70" t="s">
+      <c r="B56" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="C56" s="69"/>
-      <c r="D56" s="69"/>
-      <c r="E56" s="69"/>
-      <c r="F56" s="69"/>
-      <c r="G56" s="69"/>
-      <c r="H56" s="69"/>
+      <c r="C56" s="75"/>
+      <c r="D56" s="75"/>
+      <c r="E56" s="75"/>
+      <c r="F56" s="75"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="75"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -4344,16 +4339,16 @@
       <c r="B64" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="C64" s="72" t="s">
+      <c r="C64" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="69"/>
-      <c r="E64" s="71" t="s">
+      <c r="D64" s="75"/>
+      <c r="E64" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="F64" s="69"/>
-      <c r="G64" s="69"/>
-      <c r="H64" s="69"/>
+      <c r="F64" s="75"/>
+      <c r="G64" s="75"/>
+      <c r="H64" s="75"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -4377,15 +4372,15 @@
       <c r="A65" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="68" t="s">
+      <c r="B65" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="C65" s="69"/>
-      <c r="D65" s="69"/>
-      <c r="E65" s="69"/>
-      <c r="F65" s="69"/>
-      <c r="G65" s="69"/>
-      <c r="H65" s="69"/>
+      <c r="C65" s="75"/>
+      <c r="D65" s="75"/>
+      <c r="E65" s="75"/>
+      <c r="F65" s="75"/>
+      <c r="G65" s="75"/>
+      <c r="H65" s="75"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -4409,15 +4404,15 @@
       <c r="A66" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B66" s="70" t="s">
+      <c r="B66" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="C66" s="69"/>
-      <c r="D66" s="69"/>
-      <c r="E66" s="69"/>
-      <c r="F66" s="69"/>
-      <c r="G66" s="69"/>
-      <c r="H66" s="69"/>
+      <c r="C66" s="75"/>
+      <c r="D66" s="75"/>
+      <c r="E66" s="75"/>
+      <c r="F66" s="75"/>
+      <c r="G66" s="75"/>
+      <c r="H66" s="75"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -4630,7 +4625,7 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="90" t="s">
+      <c r="A72" s="56" t="s">
         <v>181</v>
       </c>
       <c r="B72" s="56" t="s">
@@ -4666,10 +4661,10 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="51" t="s">
+      <c r="A73" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="B73" s="51" t="s">
+      <c r="B73" s="68" t="s">
         <v>139</v>
       </c>
       <c r="C73" s="43"/>
@@ -4679,7 +4674,7 @@
       <c r="E73" s="30"/>
       <c r="F73" s="30"/>
       <c r="G73" s="30"/>
-      <c r="H73" s="67" t="s">
+      <c r="H73" s="68" t="s">
         <v>186</v>
       </c>
       <c r="I73" s="2"/>
@@ -4736,16 +4731,16 @@
       <c r="B75" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="72" t="s">
+      <c r="C75" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="D75" s="69"/>
-      <c r="E75" s="71" t="s">
+      <c r="D75" s="75"/>
+      <c r="E75" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="F75" s="69"/>
-      <c r="G75" s="69"/>
-      <c r="H75" s="69"/>
+      <c r="F75" s="75"/>
+      <c r="G75" s="75"/>
+      <c r="H75" s="75"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
@@ -4769,15 +4764,15 @@
       <c r="A76" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B76" s="68" t="s">
+      <c r="B76" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="C76" s="69"/>
-      <c r="D76" s="69"/>
-      <c r="E76" s="69"/>
-      <c r="F76" s="69"/>
-      <c r="G76" s="69"/>
-      <c r="H76" s="69"/>
+      <c r="C76" s="75"/>
+      <c r="D76" s="75"/>
+      <c r="E76" s="75"/>
+      <c r="F76" s="75"/>
+      <c r="G76" s="75"/>
+      <c r="H76" s="75"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -4801,15 +4796,15 @@
       <c r="A77" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B77" s="70" t="s">
+      <c r="B77" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="C77" s="69"/>
-      <c r="D77" s="69"/>
-      <c r="E77" s="69"/>
-      <c r="F77" s="69"/>
-      <c r="G77" s="69"/>
-      <c r="H77" s="69"/>
+      <c r="C77" s="75"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="75"/>
+      <c r="F77" s="75"/>
+      <c r="G77" s="75"/>
+      <c r="H77" s="75"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
@@ -5260,16 +5255,16 @@
       <c r="B90" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C90" s="72" t="s">
+      <c r="C90" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="D90" s="69"/>
-      <c r="E90" s="71" t="s">
+      <c r="D90" s="75"/>
+      <c r="E90" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="F90" s="69"/>
-      <c r="G90" s="69"/>
-      <c r="H90" s="69"/>
+      <c r="F90" s="75"/>
+      <c r="G90" s="75"/>
+      <c r="H90" s="75"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
@@ -5293,15 +5288,15 @@
       <c r="A91" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="68" t="s">
+      <c r="B91" s="74" t="s">
         <v>170</v>
       </c>
-      <c r="C91" s="69"/>
-      <c r="D91" s="69"/>
-      <c r="E91" s="69"/>
-      <c r="F91" s="69"/>
-      <c r="G91" s="69"/>
-      <c r="H91" s="69"/>
+      <c r="C91" s="75"/>
+      <c r="D91" s="75"/>
+      <c r="E91" s="75"/>
+      <c r="F91" s="75"/>
+      <c r="G91" s="75"/>
+      <c r="H91" s="75"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
@@ -5325,15 +5320,15 @@
       <c r="A92" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B92" s="68" t="s">
+      <c r="B92" s="74" t="s">
         <v>165</v>
       </c>
-      <c r="C92" s="69"/>
-      <c r="D92" s="69"/>
-      <c r="E92" s="69"/>
-      <c r="F92" s="69"/>
-      <c r="G92" s="69"/>
-      <c r="H92" s="69"/>
+      <c r="C92" s="75"/>
+      <c r="D92" s="75"/>
+      <c r="E92" s="75"/>
+      <c r="F92" s="75"/>
+      <c r="G92" s="75"/>
+      <c r="H92" s="75"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
@@ -5534,16 +5529,16 @@
       <c r="B98" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C98" s="84" t="s">
+      <c r="C98" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D98" s="85"/>
-      <c r="E98" s="86" t="s">
+      <c r="D98" s="78"/>
+      <c r="E98" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="F98" s="85"/>
-      <c r="G98" s="85"/>
-      <c r="H98" s="85"/>
+      <c r="F98" s="78"/>
+      <c r="G98" s="78"/>
+      <c r="H98" s="78"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
@@ -5567,15 +5562,15 @@
       <c r="A99" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B99" s="68" t="s">
+      <c r="B99" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="C99" s="69"/>
-      <c r="D99" s="69"/>
-      <c r="E99" s="69"/>
-      <c r="F99" s="69"/>
-      <c r="G99" s="69"/>
-      <c r="H99" s="69"/>
+      <c r="C99" s="75"/>
+      <c r="D99" s="75"/>
+      <c r="E99" s="75"/>
+      <c r="F99" s="75"/>
+      <c r="G99" s="75"/>
+      <c r="H99" s="75"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
@@ -5599,15 +5594,15 @@
       <c r="A100" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B100" s="68" t="s">
+      <c r="B100" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="C100" s="69"/>
-      <c r="D100" s="69"/>
-      <c r="E100" s="69"/>
-      <c r="F100" s="69"/>
-      <c r="G100" s="69"/>
-      <c r="H100" s="69"/>
+      <c r="C100" s="75"/>
+      <c r="D100" s="75"/>
+      <c r="E100" s="75"/>
+      <c r="F100" s="75"/>
+      <c r="G100" s="75"/>
+      <c r="H100" s="75"/>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
@@ -5846,16 +5841,16 @@
       <c r="B107" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C107" s="73" t="s">
+      <c r="C107" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="D107" s="74"/>
-      <c r="E107" s="75" t="s">
+      <c r="D107" s="72"/>
+      <c r="E107" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="F107" s="74"/>
-      <c r="G107" s="74"/>
-      <c r="H107" s="74"/>
+      <c r="F107" s="72"/>
+      <c r="G107" s="72"/>
+      <c r="H107" s="72"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
@@ -5871,15 +5866,15 @@
       <c r="A108" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="87" t="s">
+      <c r="B108" s="80" t="s">
         <v>144</v>
       </c>
-      <c r="C108" s="88"/>
-      <c r="D108" s="88"/>
-      <c r="E108" s="88"/>
-      <c r="F108" s="88"/>
-      <c r="G108" s="88"/>
-      <c r="H108" s="89"/>
+      <c r="C108" s="81"/>
+      <c r="D108" s="81"/>
+      <c r="E108" s="81"/>
+      <c r="F108" s="81"/>
+      <c r="G108" s="81"/>
+      <c r="H108" s="82"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
@@ -5895,15 +5890,15 @@
       <c r="A109" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="82" t="s">
+      <c r="B109" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="C109" s="83"/>
-      <c r="D109" s="83"/>
-      <c r="E109" s="83"/>
-      <c r="F109" s="83"/>
-      <c r="G109" s="83"/>
-      <c r="H109" s="83"/>
+      <c r="C109" s="70"/>
+      <c r="D109" s="70"/>
+      <c r="E109" s="70"/>
+      <c r="F109" s="70"/>
+      <c r="G109" s="70"/>
+      <c r="H109" s="70"/>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
@@ -8421,36 +8416,6 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B109:H109"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="E107:H107"/>
-    <mergeCell ref="B99:H99"/>
-    <mergeCell ref="B77:H77"/>
-    <mergeCell ref="B100:H100"/>
-    <mergeCell ref="B92:H92"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="E98:H98"/>
-    <mergeCell ref="B108:H108"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:H54"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B55:H55"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="E75:H75"/>
-    <mergeCell ref="B76:H76"/>
-    <mergeCell ref="B91:H91"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:H64"/>
-    <mergeCell ref="B65:H65"/>
-    <mergeCell ref="B66:H66"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="E21:H21"/>
@@ -8467,6 +8432,36 @@
     <mergeCell ref="E36:H36"/>
     <mergeCell ref="B37:H37"/>
     <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B76:H76"/>
+    <mergeCell ref="B91:H91"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="E64:H64"/>
+    <mergeCell ref="B65:H65"/>
+    <mergeCell ref="B66:H66"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:H54"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="E75:H75"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B109:H109"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="E107:H107"/>
+    <mergeCell ref="B99:H99"/>
+    <mergeCell ref="B77:H77"/>
+    <mergeCell ref="B100:H100"/>
+    <mergeCell ref="B92:H92"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="E98:H98"/>
+    <mergeCell ref="B108:H108"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MENU_CATEGORY_DELETE 추가 SALE_DATE 삭제 -> RECIEPT JOIN 해서 사용
</commit_message>
<xml_diff>
--- a/doc/ONCE_DB설계서150705.xlsx
+++ b/doc/ONCE_DB설계서150705.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="460" windowWidth="18080" windowHeight="19020"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="195">
   <si>
     <t>문서번호</t>
   </si>
@@ -787,14 +787,6 @@
   </si>
   <si>
     <t>Once</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>판매 일자</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1007,10 +999,6 @@
   </si>
   <si>
     <t>SALE_NUM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SALE_DATE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1368,6 +1356,18 @@
   </si>
   <si>
     <t>SALE Table quntity 추가, RECEIPT subtotal discount 추가, MENU WHIP 추가</t>
+  </si>
+  <si>
+    <t>MENU_CATEGORY_DELETE</t>
+  </si>
+  <si>
+    <t>메뉴 삭제 유무 Y or N</t>
+  </si>
+  <si>
+    <t>N'</t>
+  </si>
+  <si>
+    <t>MENU_CATEGORY_DELETE 추가, SALE_DATE 삭제 -&gt; RECIEPT JOIN 해서 사용</t>
   </si>
 </sst>
 </file>
@@ -1623,7 +1623,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1761,14 +1761,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1776,9 +1780,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1795,26 +1812,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준 2" xfId="1"/>
@@ -2150,8 +2151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2164,18 +2165,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="76" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -2196,15 +2197,15 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="84"/>
+      <c r="A2" s="77"/>
       <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
       <c r="F2" s="24" t="s">
         <v>2</v>
       </c>
@@ -2232,15 +2233,15 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="84"/>
+      <c r="A3" s="77"/>
       <c r="B3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="24" t="s">
         <v>5</v>
       </c>
@@ -2296,18 +2297,18 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="65">
+      <c r="A5" s="91">
         <v>42190</v>
       </c>
-      <c r="B5" s="90" t="s">
-        <v>179</v>
-      </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
+      <c r="B5" s="81" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2328,18 +2329,18 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="65">
+      <c r="A6" s="91">
         <v>42232</v>
       </c>
-      <c r="B6" s="90" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
+      <c r="B6" s="81" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -2360,7 +2361,18 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="44"/>
+      <c r="A7" s="91">
+        <v>42250</v>
+      </c>
+      <c r="B7" s="90" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -2415,16 +2427,16 @@
       <c r="B9" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="89" t="s">
+      <c r="C9" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="75"/>
-      <c r="E9" s="88" t="s">
+      <c r="D9" s="69"/>
+      <c r="E9" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2448,15 +2460,15 @@
       <c r="A10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -2480,15 +2492,15 @@
       <c r="A11" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="70" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -2823,16 +2835,16 @@
       <c r="B21" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="75"/>
-      <c r="E21" s="88" t="s">
+      <c r="D21" s="69"/>
+      <c r="E21" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -2856,15 +2868,15 @@
       <c r="A22" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="74" t="s">
+      <c r="B22" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="75"/>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -2888,15 +2900,15 @@
       <c r="A23" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="75"/>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -3000,7 +3012,7 @@
     </row>
     <row r="26" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B26" s="51" t="s">
         <v>119</v>
@@ -3036,7 +3048,7 @@
     </row>
     <row r="27" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="45" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B27" s="45" t="s">
         <v>60</v>
@@ -3087,7 +3099,7 @@
       <c r="F28" s="30"/>
       <c r="G28" s="30"/>
       <c r="H28" s="47" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -3123,7 +3135,7 @@
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
       <c r="H29" s="47" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -3145,11 +3157,11 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="66" t="s">
-        <v>187</v>
-      </c>
-      <c r="B30" s="66" t="s">
-        <v>188</v>
+      <c r="A30" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" s="65" t="s">
+        <v>185</v>
       </c>
       <c r="C30" s="43">
         <v>1</v>
@@ -3158,10 +3170,10 @@
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
       <c r="G30" s="61" t="s">
+        <v>186</v>
+      </c>
+      <c r="H30" s="66" t="s">
         <v>189</v>
-      </c>
-      <c r="H30" s="67" t="s">
-        <v>192</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -3256,7 +3268,7 @@
     </row>
     <row r="33" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="51" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B33" s="51" t="s">
         <v>121</v>
@@ -3294,7 +3306,7 @@
     </row>
     <row r="34" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="45" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B34" s="45" t="s">
         <v>25</v>
@@ -3309,7 +3321,7 @@
       </c>
       <c r="G34" s="30"/>
       <c r="H34" s="62" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -3365,16 +3377,16 @@
       <c r="B36" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="C36" s="89" t="s">
+      <c r="C36" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="75"/>
-      <c r="E36" s="88" t="s">
+      <c r="D36" s="69"/>
+      <c r="E36" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="F36" s="75"/>
-      <c r="G36" s="75"/>
-      <c r="H36" s="75"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -3398,15 +3410,15 @@
       <c r="A37" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="74" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="75"/>
+      <c r="B37" s="68" t="s">
+        <v>149</v>
+      </c>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -3430,15 +3442,15 @@
       <c r="A38" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="74" t="s">
+      <c r="B38" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="75"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="75"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -3502,7 +3514,7 @@
     </row>
     <row r="40" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="33" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B40" s="51" t="s">
         <v>17</v>
@@ -3555,7 +3567,7 @@
       </c>
       <c r="G41" s="30"/>
       <c r="H41" s="51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -3578,7 +3590,7 @@
     </row>
     <row r="42" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>32</v>
@@ -3677,16 +3689,16 @@
       <c r="B45" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="C45" s="71" t="s">
+      <c r="C45" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="72"/>
-      <c r="E45" s="73" t="s">
+      <c r="D45" s="74"/>
+      <c r="E45" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
-      <c r="H45" s="72"/>
+      <c r="F45" s="74"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="74"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
@@ -3710,15 +3722,15 @@
       <c r="A46" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="74" t="s">
-        <v>152</v>
-      </c>
-      <c r="C46" s="75"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="75"/>
-      <c r="H46" s="75"/>
+      <c r="B46" s="68" t="s">
+        <v>150</v>
+      </c>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="69"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -3742,15 +3754,15 @@
       <c r="A47" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="76" t="s">
+      <c r="B47" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="75"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
@@ -3814,7 +3826,7 @@
     </row>
     <row r="49" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>35</v>
@@ -3852,7 +3864,7 @@
     </row>
     <row r="50" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>21</v>
@@ -3889,14 +3901,24 @@
       <c r="Z50" s="2"/>
     </row>
     <row r="51" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="10"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="11"/>
+      <c r="A51" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C51" s="11">
+        <v>1</v>
+      </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="5"/>
+      <c r="G51" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -3979,16 +4001,16 @@
       <c r="B54" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="C54" s="89" t="s">
+      <c r="C54" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="75"/>
-      <c r="E54" s="88" t="s">
+      <c r="D54" s="69"/>
+      <c r="E54" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="F54" s="75"/>
-      <c r="G54" s="75"/>
-      <c r="H54" s="75"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="69"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -4012,15 +4034,15 @@
       <c r="A55" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="74" t="s">
-        <v>158</v>
-      </c>
-      <c r="C55" s="75"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="75"/>
+      <c r="B55" s="68" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
+      <c r="F55" s="69"/>
+      <c r="G55" s="69"/>
+      <c r="H55" s="69"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -4044,15 +4066,15 @@
       <c r="A56" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B56" s="76" t="s">
+      <c r="B56" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="C56" s="75"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="75"/>
-      <c r="F56" s="75"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="75"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="69"/>
+      <c r="F56" s="69"/>
+      <c r="G56" s="69"/>
+      <c r="H56" s="69"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -4118,7 +4140,7 @@
     </row>
     <row r="58" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>17</v>
@@ -4156,7 +4178,7 @@
     </row>
     <row r="59" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>35</v>
@@ -4171,7 +4193,7 @@
       </c>
       <c r="G59" s="9"/>
       <c r="H59" s="63" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -4194,22 +4216,22 @@
     </row>
     <row r="60" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G60" s="9"/>
+      <c r="H60" s="64" t="s">
         <v>160</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="17" t="s">
-        <v>127</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -4232,22 +4254,20 @@
     </row>
     <row r="61" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="10" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="C61" s="11"/>
-      <c r="D61" s="9" t="s">
-        <v>116</v>
-      </c>
+      <c r="D61" s="9"/>
       <c r="E61" s="9"/>
-      <c r="F61" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="G61" s="9"/>
-      <c r="H61" s="64" t="s">
-        <v>163</v>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9">
+        <v>1</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>177</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -4269,22 +4289,14 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" s="11"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9">
-        <v>1</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>180</v>
-      </c>
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="58"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -4305,14 +4317,22 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="58"/>
+      <c r="A63" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="C63" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="69"/>
+      <c r="E63" s="71" t="s">
+        <v>124</v>
+      </c>
+      <c r="F63" s="69"/>
+      <c r="G63" s="69"/>
+      <c r="H63" s="69"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
@@ -4334,21 +4354,17 @@
     </row>
     <row r="64" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B64" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="C64" s="89" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" s="75"/>
-      <c r="E64" s="88" t="s">
-        <v>124</v>
-      </c>
-      <c r="F64" s="75"/>
-      <c r="G64" s="75"/>
-      <c r="H64" s="75"/>
+        <v>8</v>
+      </c>
+      <c r="B64" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" s="69"/>
+      <c r="D64" s="69"/>
+      <c r="E64" s="69"/>
+      <c r="F64" s="69"/>
+      <c r="G64" s="69"/>
+      <c r="H64" s="69"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -4370,17 +4386,17 @@
     </row>
     <row r="65" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="74" t="s">
-        <v>157</v>
-      </c>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="75"/>
-      <c r="H65" s="75"/>
+        <v>9</v>
+      </c>
+      <c r="B65" s="70" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" s="69"/>
+      <c r="D65" s="69"/>
+      <c r="E65" s="69"/>
+      <c r="F65" s="69"/>
+      <c r="G65" s="69"/>
+      <c r="H65" s="69"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -4402,17 +4418,29 @@
     </row>
     <row r="66" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="B66" s="76" t="s">
-        <v>129</v>
-      </c>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="75"/>
+        <v>10</v>
+      </c>
+      <c r="B66" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="H66" s="50" t="s">
+        <v>16</v>
+      </c>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -4433,29 +4461,23 @@
       <c r="Z66" s="2"/>
     </row>
     <row r="67" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="D67" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E67" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="F67" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="G67" s="50" t="s">
-        <v>26</v>
-      </c>
-      <c r="H67" s="50" t="s">
-        <v>16</v>
+      <c r="A67" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B67" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="29"/>
+      <c r="D67" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" s="30"/>
+      <c r="G67" s="30"/>
+      <c r="H67" s="51" t="s">
+        <v>37</v>
       </c>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
@@ -4478,22 +4500,20 @@
     </row>
     <row r="68" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" s="51" t="s">
         <v>130</v>
-      </c>
-      <c r="B68" s="51" t="s">
-        <v>17</v>
       </c>
       <c r="C68" s="29"/>
       <c r="D68" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="30" t="s">
-        <v>18</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E68" s="30"/>
       <c r="F68" s="30"/>
       <c r="G68" s="30"/>
-      <c r="H68" s="51" t="s">
-        <v>37</v>
+      <c r="H68" s="49" t="s">
+        <v>132</v>
       </c>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
@@ -4515,21 +4535,23 @@
       <c r="Z68" s="2"/>
     </row>
     <row r="69" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="33" t="s">
-        <v>131</v>
+      <c r="A69" s="65" t="s">
+        <v>144</v>
       </c>
       <c r="B69" s="51" t="s">
-        <v>132</v>
-      </c>
-      <c r="C69" s="29"/>
+        <v>133</v>
+      </c>
+      <c r="C69" s="43">
+        <v>1</v>
+      </c>
       <c r="D69" s="30" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E69" s="30"/>
       <c r="F69" s="30"/>
-      <c r="G69" s="30"/>
+      <c r="G69" s="61"/>
       <c r="H69" s="49" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
@@ -4551,23 +4573,21 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="66" t="s">
-        <v>146</v>
-      </c>
-      <c r="B70" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="C70" s="43">
-        <v>1</v>
-      </c>
-      <c r="D70" s="30" t="s">
-        <v>136</v>
-      </c>
+      <c r="A70" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B70" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" s="43"/>
+      <c r="D70" s="30"/>
       <c r="E70" s="30"/>
       <c r="F70" s="30"/>
-      <c r="G70" s="61"/>
-      <c r="H70" s="49" t="s">
-        <v>137</v>
+      <c r="G70" s="61">
+        <v>0</v>
+      </c>
+      <c r="H70" s="29" t="s">
+        <v>182</v>
       </c>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
@@ -4589,21 +4609,21 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="B71" s="29" t="s">
+      <c r="A71" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="B71" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C71" s="43"/>
-      <c r="D71" s="30"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
-      <c r="G71" s="61">
-        <v>0</v>
-      </c>
-      <c r="H71" s="29" t="s">
-        <v>185</v>
+      <c r="C71" s="56"/>
+      <c r="D71" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="57"/>
+      <c r="F71" s="57"/>
+      <c r="G71" s="57"/>
+      <c r="H71" s="56" t="s">
+        <v>180</v>
       </c>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
@@ -4625,20 +4645,20 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="56" t="s">
-        <v>181</v>
-      </c>
-      <c r="B72" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="C72" s="56"/>
-      <c r="D72" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="E72" s="57"/>
-      <c r="F72" s="57"/>
-      <c r="G72" s="57"/>
-      <c r="H72" s="56" t="s">
+      <c r="A72" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="C72" s="43"/>
+      <c r="D72" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E72" s="30"/>
+      <c r="F72" s="30"/>
+      <c r="G72" s="30"/>
+      <c r="H72" s="67" t="s">
         <v>183</v>
       </c>
       <c r="I72" s="2"/>
@@ -4661,22 +4681,14 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="68" t="s">
-        <v>138</v>
-      </c>
-      <c r="B73" s="68" t="s">
-        <v>139</v>
-      </c>
-      <c r="C73" s="43"/>
-      <c r="D73" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
-      <c r="G73" s="30"/>
-      <c r="H73" s="68" t="s">
-        <v>186</v>
-      </c>
+      <c r="A73" s="3"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
@@ -4697,14 +4709,22 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="3"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="2"/>
+      <c r="A74" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C74" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="69"/>
+      <c r="E74" s="71" t="s">
+        <v>124</v>
+      </c>
+      <c r="F74" s="69"/>
+      <c r="G74" s="69"/>
+      <c r="H74" s="69"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
@@ -4726,21 +4746,17 @@
     </row>
     <row r="75" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B75" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="C75" s="89" t="s">
-        <v>7</v>
-      </c>
-      <c r="D75" s="75"/>
-      <c r="E75" s="88" t="s">
-        <v>124</v>
-      </c>
-      <c r="F75" s="75"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
+        <v>8</v>
+      </c>
+      <c r="B75" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75" s="69"/>
+      <c r="D75" s="69"/>
+      <c r="E75" s="69"/>
+      <c r="F75" s="69"/>
+      <c r="G75" s="69"/>
+      <c r="H75" s="69"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
@@ -4762,17 +4778,17 @@
     </row>
     <row r="76" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B76" s="74" t="s">
-        <v>167</v>
-      </c>
-      <c r="C76" s="75"/>
-      <c r="D76" s="75"/>
-      <c r="E76" s="75"/>
-      <c r="F76" s="75"/>
-      <c r="G76" s="75"/>
-      <c r="H76" s="75"/>
+        <v>9</v>
+      </c>
+      <c r="B76" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" s="69"/>
+      <c r="D76" s="69"/>
+      <c r="E76" s="69"/>
+      <c r="F76" s="69"/>
+      <c r="G76" s="69"/>
+      <c r="H76" s="69"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -4793,18 +4809,28 @@
       <c r="Z76" s="2"/>
     </row>
     <row r="77" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B77" s="76" t="s">
-        <v>77</v>
-      </c>
-      <c r="C77" s="75"/>
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
-      <c r="F77" s="75"/>
-      <c r="G77" s="75"/>
-      <c r="H77" s="75"/>
+      <c r="A77" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18" t="s">
+        <v>16</v>
+      </c>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
@@ -4825,27 +4851,23 @@
       <c r="Z77" s="2"/>
     </row>
     <row r="78" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="54" t="s">
-        <v>10</v>
-      </c>
-      <c r="B78" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C78" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D78" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E78" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G78" s="18"/>
-      <c r="H78" s="18" t="s">
-        <v>16</v>
+      <c r="A78" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="B78" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78" s="46"/>
+      <c r="D78" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="47" t="s">
+        <v>34</v>
       </c>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
@@ -4868,22 +4890,22 @@
     </row>
     <row r="79" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="45" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B79" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="C79" s="46"/>
+        <v>78</v>
+      </c>
+      <c r="C79" s="46">
+        <v>150</v>
+      </c>
       <c r="D79" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E79" s="19" t="s">
-        <v>23</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E79" s="19"/>
       <c r="F79" s="19"/>
       <c r="G79" s="19"/>
       <c r="H79" s="47" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
@@ -4906,13 +4928,13 @@
     </row>
     <row r="80" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="45" t="s">
-        <v>168</v>
+        <v>80</v>
       </c>
       <c r="B80" s="46" t="s">
         <v>78</v>
       </c>
       <c r="C80" s="46">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D80" s="19" t="s">
         <v>50</v>
@@ -4921,7 +4943,7 @@
       <c r="F80" s="19"/>
       <c r="G80" s="19"/>
       <c r="H80" s="47" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
@@ -4944,22 +4966,22 @@
     </row>
     <row r="81" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="45" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="B81" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="C81" s="46">
-        <v>300</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C81" s="46"/>
       <c r="D81" s="19" t="s">
         <v>50</v>
       </c>
       <c r="E81" s="19"/>
-      <c r="F81" s="19"/>
+      <c r="F81" s="19" t="s">
+        <v>85</v>
+      </c>
       <c r="G81" s="19"/>
       <c r="H81" s="47" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
@@ -4982,22 +5004,20 @@
     </row>
     <row r="82" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="45" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="B82" s="46" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C82" s="46"/>
       <c r="D82" s="19" t="s">
         <v>50</v>
       </c>
       <c r="E82" s="19"/>
-      <c r="F82" s="19" t="s">
-        <v>85</v>
-      </c>
+      <c r="F82" s="19"/>
       <c r="G82" s="19"/>
       <c r="H82" s="47" t="s">
-        <v>169</v>
+        <v>87</v>
       </c>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
@@ -5020,20 +5040,20 @@
     </row>
     <row r="83" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="45" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="B83" s="46" t="s">
         <v>86</v>
       </c>
       <c r="C83" s="46"/>
-      <c r="D83" s="19" t="s">
-        <v>50</v>
-      </c>
+      <c r="D83" s="19"/>
       <c r="E83" s="19"/>
       <c r="F83" s="19"/>
-      <c r="G83" s="19"/>
+      <c r="G83" s="19">
+        <v>0</v>
+      </c>
       <c r="H83" s="47" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
@@ -5056,10 +5076,10 @@
     </row>
     <row r="84" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="45" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B84" s="46" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C84" s="46"/>
       <c r="D84" s="19"/>
@@ -5069,7 +5089,7 @@
         <v>0</v>
       </c>
       <c r="H84" s="47" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
@@ -5092,20 +5112,22 @@
     </row>
     <row r="85" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="45" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B85" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="C85" s="46"/>
+        <v>92</v>
+      </c>
+      <c r="C85" s="46">
+        <v>1</v>
+      </c>
       <c r="D85" s="19"/>
       <c r="E85" s="19"/>
       <c r="F85" s="19"/>
-      <c r="G85" s="19">
-        <v>0</v>
+      <c r="G85" s="59" t="s">
+        <v>93</v>
       </c>
       <c r="H85" s="47" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
@@ -5127,24 +5149,14 @@
       <c r="Z85" s="2"/>
     </row>
     <row r="86" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="45" t="s">
-        <v>91</v>
-      </c>
-      <c r="B86" s="46" t="s">
-        <v>92</v>
-      </c>
-      <c r="C86" s="46">
-        <v>1</v>
-      </c>
-      <c r="D86" s="19"/>
-      <c r="E86" s="19"/>
-      <c r="F86" s="19"/>
-      <c r="G86" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="H86" s="47" t="s">
-        <v>94</v>
-      </c>
+      <c r="A86" s="45"/>
+      <c r="B86" s="45"/>
+      <c r="C86" s="43"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="30"/>
+      <c r="F86" s="30"/>
+      <c r="G86" s="30"/>
+      <c r="H86" s="45"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
@@ -5165,14 +5177,14 @@
       <c r="Z86" s="2"/>
     </row>
     <row r="87" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="45"/>
-      <c r="B87" s="45"/>
-      <c r="C87" s="43"/>
-      <c r="D87" s="30"/>
-      <c r="E87" s="30"/>
-      <c r="F87" s="30"/>
-      <c r="G87" s="30"/>
-      <c r="H87" s="45"/>
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="2"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
@@ -5193,7 +5205,7 @@
       <c r="Z87" s="2"/>
     </row>
     <row r="88" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="2"/>
+      <c r="A88" s="3"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="14"/>
@@ -5221,14 +5233,22 @@
       <c r="Z88" s="2"/>
     </row>
     <row r="89" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="3"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="2"/>
+      <c r="A89" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C89" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" s="69"/>
+      <c r="E89" s="71" t="s">
+        <v>124</v>
+      </c>
+      <c r="F89" s="69"/>
+      <c r="G89" s="69"/>
+      <c r="H89" s="69"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
@@ -5250,21 +5270,17 @@
     </row>
     <row r="90" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B90" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C90" s="89" t="s">
-        <v>7</v>
-      </c>
-      <c r="D90" s="75"/>
-      <c r="E90" s="88" t="s">
-        <v>124</v>
-      </c>
-      <c r="F90" s="75"/>
-      <c r="G90" s="75"/>
-      <c r="H90" s="75"/>
+        <v>8</v>
+      </c>
+      <c r="B90" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="C90" s="69"/>
+      <c r="D90" s="69"/>
+      <c r="E90" s="69"/>
+      <c r="F90" s="69"/>
+      <c r="G90" s="69"/>
+      <c r="H90" s="69"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
@@ -5286,17 +5302,17 @@
     </row>
     <row r="91" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B91" s="74" t="s">
-        <v>170</v>
-      </c>
-      <c r="C91" s="75"/>
-      <c r="D91" s="75"/>
-      <c r="E91" s="75"/>
-      <c r="F91" s="75"/>
-      <c r="G91" s="75"/>
-      <c r="H91" s="75"/>
+        <v>9</v>
+      </c>
+      <c r="B91" s="68" t="s">
+        <v>162</v>
+      </c>
+      <c r="C91" s="69"/>
+      <c r="D91" s="69"/>
+      <c r="E91" s="69"/>
+      <c r="F91" s="69"/>
+      <c r="G91" s="69"/>
+      <c r="H91" s="69"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
@@ -5317,18 +5333,28 @@
       <c r="Z91" s="2"/>
     </row>
     <row r="92" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B92" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="C92" s="75"/>
-      <c r="D92" s="75"/>
-      <c r="E92" s="75"/>
-      <c r="F92" s="75"/>
-      <c r="G92" s="75"/>
-      <c r="H92" s="75"/>
+      <c r="A92" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
@@ -5349,27 +5375,23 @@
       <c r="Z92" s="2"/>
     </row>
     <row r="93" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B93" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G93" s="6"/>
-      <c r="H93" s="6" t="s">
-        <v>16</v>
+      <c r="A93" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
@@ -5391,23 +5413,23 @@
       <c r="Z93" s="2"/>
     </row>
     <row r="94" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="7" t="s">
-        <v>141</v>
+      <c r="A94" s="10" t="s">
+        <v>168</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C94" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="C94" s="8">
+        <v>50</v>
+      </c>
       <c r="D94" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>18</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E94" s="9"/>
       <c r="F94" s="9"/>
       <c r="G94" s="9"/>
       <c r="H94" s="5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
@@ -5429,24 +5451,14 @@
       <c r="Z94" s="2"/>
     </row>
     <row r="95" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C95" s="8">
-        <v>50</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E95" s="9"/>
-      <c r="F95" s="9"/>
-      <c r="G95" s="9"/>
-      <c r="H95" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
@@ -5467,14 +5479,14 @@
       <c r="Z95" s="2"/>
     </row>
     <row r="96" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="2"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="14"/>
-      <c r="E96" s="14"/>
-      <c r="F96" s="14"/>
-      <c r="G96" s="14"/>
-      <c r="H96" s="2"/>
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="3"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -5495,14 +5507,22 @@
       <c r="Z96" s="2"/>
     </row>
     <row r="97" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="13"/>
-      <c r="E97" s="13"/>
-      <c r="F97" s="13"/>
-      <c r="G97" s="13"/>
-      <c r="H97" s="3"/>
+      <c r="A97" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C97" s="84" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" s="85"/>
+      <c r="E97" s="86" t="s">
+        <v>124</v>
+      </c>
+      <c r="F97" s="85"/>
+      <c r="G97" s="85"/>
+      <c r="H97" s="85"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
@@ -5523,22 +5543,18 @@
       <c r="Z97" s="2"/>
     </row>
     <row r="98" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B98" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C98" s="77" t="s">
-        <v>7</v>
-      </c>
-      <c r="D98" s="78"/>
-      <c r="E98" s="79" t="s">
-        <v>124</v>
-      </c>
-      <c r="F98" s="78"/>
-      <c r="G98" s="78"/>
-      <c r="H98" s="78"/>
+      <c r="A98" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="68" t="s">
+        <v>170</v>
+      </c>
+      <c r="C98" s="69"/>
+      <c r="D98" s="69"/>
+      <c r="E98" s="69"/>
+      <c r="F98" s="69"/>
+      <c r="G98" s="69"/>
+      <c r="H98" s="69"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
@@ -5560,17 +5576,17 @@
     </row>
     <row r="99" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B99" s="74" t="s">
-        <v>173</v>
-      </c>
-      <c r="C99" s="75"/>
-      <c r="D99" s="75"/>
-      <c r="E99" s="75"/>
-      <c r="F99" s="75"/>
-      <c r="G99" s="75"/>
-      <c r="H99" s="75"/>
+        <v>9</v>
+      </c>
+      <c r="B99" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="C99" s="69"/>
+      <c r="D99" s="69"/>
+      <c r="E99" s="69"/>
+      <c r="F99" s="69"/>
+      <c r="G99" s="69"/>
+      <c r="H99" s="69"/>
       <c r="I99" s="2"/>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
@@ -5591,18 +5607,28 @@
       <c r="Z99" s="2"/>
     </row>
     <row r="100" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B100" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="C100" s="75"/>
-      <c r="D100" s="75"/>
-      <c r="E100" s="75"/>
-      <c r="F100" s="75"/>
-      <c r="G100" s="75"/>
-      <c r="H100" s="75"/>
+      <c r="A100" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="I100" s="2"/>
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
@@ -5623,27 +5649,23 @@
       <c r="Z100" s="2"/>
     </row>
     <row r="101" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B101" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F101" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G101" s="6"/>
-      <c r="H101" s="6" t="s">
-        <v>16</v>
+      <c r="A101" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C101" s="8"/>
+      <c r="D101" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
@@ -5665,23 +5687,23 @@
       <c r="Z101" s="2"/>
     </row>
     <row r="102" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B102" s="5" t="s">
+      <c r="A102" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B102" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C102" s="8"/>
-      <c r="D102" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F102" s="9"/>
-      <c r="G102" s="9"/>
-      <c r="H102" s="5" t="s">
-        <v>19</v>
+      <c r="C102" s="32"/>
+      <c r="D102" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G102" s="27"/>
+      <c r="H102" s="25" t="s">
+        <v>175</v>
       </c>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
@@ -5703,23 +5725,23 @@
       <c r="Z102" s="2"/>
     </row>
     <row r="103" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B103" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C103" s="32"/>
-      <c r="D103" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E103" s="27"/>
-      <c r="F103" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="G103" s="27"/>
-      <c r="H103" s="25" t="s">
-        <v>178</v>
+      <c r="A103" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B103" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C103" s="29">
+        <v>255</v>
+      </c>
+      <c r="D103" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E103" s="30"/>
+      <c r="F103" s="30"/>
+      <c r="G103" s="30"/>
+      <c r="H103" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
@@ -5741,24 +5763,14 @@
       <c r="Z103" s="2"/>
     </row>
     <row r="104" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="B104" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C104" s="29">
-        <v>255</v>
-      </c>
-      <c r="D104" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="E104" s="30"/>
-      <c r="F104" s="30"/>
-      <c r="G104" s="30"/>
-      <c r="H104" s="29" t="s">
-        <v>33</v>
-      </c>
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="2"/>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
@@ -5807,14 +5819,22 @@
       <c r="Z105" s="2"/>
     </row>
     <row r="106" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="2"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14"/>
-      <c r="G106" s="14"/>
-      <c r="H106" s="2"/>
+      <c r="A106" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C106" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106" s="74"/>
+      <c r="E106" s="75" t="s">
+        <v>124</v>
+      </c>
+      <c r="F106" s="74"/>
+      <c r="G106" s="74"/>
+      <c r="H106" s="74"/>
       <c r="I106" s="2"/>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
@@ -5835,22 +5855,18 @@
       <c r="Z106" s="2"/>
     </row>
     <row r="107" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B107" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C107" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="D107" s="72"/>
-      <c r="E107" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="F107" s="72"/>
-      <c r="G107" s="72"/>
-      <c r="H107" s="72"/>
+      <c r="A107" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" s="87" t="s">
+        <v>142</v>
+      </c>
+      <c r="C107" s="88"/>
+      <c r="D107" s="88"/>
+      <c r="E107" s="88"/>
+      <c r="F107" s="88"/>
+      <c r="G107" s="88"/>
+      <c r="H107" s="89"/>
       <c r="I107" s="2"/>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
@@ -5863,18 +5879,18 @@
       <c r="R107" s="2"/>
     </row>
     <row r="108" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B108" s="80" t="s">
-        <v>144</v>
-      </c>
-      <c r="C108" s="81"/>
-      <c r="D108" s="81"/>
-      <c r="E108" s="81"/>
-      <c r="F108" s="81"/>
-      <c r="G108" s="81"/>
-      <c r="H108" s="82"/>
+      <c r="A108" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B108" s="82" t="s">
+        <v>98</v>
+      </c>
+      <c r="C108" s="83"/>
+      <c r="D108" s="83"/>
+      <c r="E108" s="83"/>
+      <c r="F108" s="83"/>
+      <c r="G108" s="83"/>
+      <c r="H108" s="83"/>
       <c r="I108" s="2"/>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
@@ -5888,17 +5904,27 @@
     </row>
     <row r="109" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B109" s="69" t="s">
-        <v>98</v>
-      </c>
-      <c r="C109" s="70"/>
-      <c r="D109" s="70"/>
-      <c r="E109" s="70"/>
-      <c r="F109" s="70"/>
-      <c r="G109" s="70"/>
-      <c r="H109" s="70"/>
+        <v>10</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E109" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G109" s="20"/>
+      <c r="H109" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="I109" s="2"/>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
@@ -5911,27 +5937,23 @@
       <c r="R109" s="2"/>
     </row>
     <row r="110" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B110" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C110" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D110" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E110" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F110" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G110" s="20"/>
-      <c r="H110" s="20" t="s">
-        <v>16</v>
+      <c r="A110" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B110" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C110" s="29"/>
+      <c r="D110" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E110" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F110" s="30"/>
+      <c r="G110" s="30"/>
+      <c r="H110" s="47" t="s">
+        <v>34</v>
       </c>
       <c r="I110" s="2"/>
       <c r="J110" s="2"/>
@@ -5946,22 +5968,22 @@
     </row>
     <row r="111" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B111" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C111" s="29"/>
+        <v>101</v>
+      </c>
+      <c r="B111" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C111" s="29">
+        <v>150</v>
+      </c>
       <c r="D111" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="E111" s="30" t="s">
-        <v>100</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E111" s="30"/>
       <c r="F111" s="30"/>
       <c r="G111" s="30"/>
       <c r="H111" s="47" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
@@ -5975,23 +5997,23 @@
       <c r="R111" s="2"/>
     </row>
     <row r="112" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B112" s="37" t="s">
+      <c r="A112" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B112" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C112" s="29">
-        <v>150</v>
-      </c>
-      <c r="D112" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E112" s="30"/>
-      <c r="F112" s="30"/>
-      <c r="G112" s="30"/>
-      <c r="H112" s="47" t="s">
-        <v>102</v>
+      <c r="C112" s="8">
+        <v>300</v>
+      </c>
+      <c r="D112" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="9"/>
+      <c r="H112" s="17" t="s">
+        <v>105</v>
       </c>
       <c r="I112" s="2"/>
       <c r="J112" s="2"/>
@@ -6006,13 +6028,13 @@
     </row>
     <row r="113" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="12" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C113" s="8">
-        <v>300</v>
+        <v>255</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>18</v>
@@ -6021,7 +6043,7 @@
       <c r="F113" s="9"/>
       <c r="G113" s="9"/>
       <c r="H113" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I113" s="2"/>
       <c r="J113" s="2"/>
@@ -6036,22 +6058,24 @@
     </row>
     <row r="114" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="12" t="s">
-        <v>145</v>
+        <v>106</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C114" s="8">
-        <v>255</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C114" s="8"/>
       <c r="D114" s="9" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="E114" s="9"/>
-      <c r="F114" s="9"/>
-      <c r="G114" s="9"/>
+      <c r="F114" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G114" s="9">
+        <v>0</v>
+      </c>
       <c r="H114" s="17" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I114" s="2"/>
       <c r="J114" s="2"/>
@@ -6066,24 +6090,20 @@
     </row>
     <row r="115" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="12" t="s">
-        <v>106</v>
+        <v>174</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>89</v>
+        <v>171</v>
       </c>
       <c r="C115" s="8"/>
       <c r="D115" s="9" t="s">
-        <v>118</v>
+        <v>173</v>
       </c>
       <c r="E115" s="9"/>
-      <c r="F115" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="G115" s="9">
-        <v>0</v>
-      </c>
+      <c r="F115" s="9"/>
+      <c r="G115" s="9"/>
       <c r="H115" s="17" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="I115" s="2"/>
       <c r="J115" s="2"/>
@@ -6098,20 +6118,20 @@
     </row>
     <row r="116" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="12" t="s">
-        <v>177</v>
+        <v>108</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>174</v>
+        <v>109</v>
       </c>
       <c r="C116" s="8"/>
-      <c r="D116" s="9" t="s">
-        <v>176</v>
-      </c>
+      <c r="D116" s="9"/>
       <c r="E116" s="9"/>
       <c r="F116" s="9"/>
-      <c r="G116" s="9"/>
+      <c r="G116" s="9">
+        <v>0</v>
+      </c>
       <c r="H116" s="17" t="s">
-        <v>175</v>
+        <v>110</v>
       </c>
       <c r="I116" s="2"/>
       <c r="J116" s="2"/>
@@ -6126,20 +6146,22 @@
     </row>
     <row r="117" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="12" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C117" s="8"/>
+        <v>112</v>
+      </c>
+      <c r="C117" s="8">
+        <v>1</v>
+      </c>
       <c r="D117" s="9"/>
       <c r="E117" s="9"/>
       <c r="F117" s="9"/>
-      <c r="G117" s="9">
-        <v>0</v>
+      <c r="G117" s="16" t="s">
+        <v>113</v>
       </c>
       <c r="H117" s="17" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I117" s="2"/>
       <c r="J117" s="2"/>
@@ -6153,24 +6175,14 @@
       <c r="R117" s="2"/>
     </row>
     <row r="118" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C118" s="8">
-        <v>1</v>
-      </c>
+      <c r="A118" s="12"/>
+      <c r="B118" s="5"/>
+      <c r="C118" s="8"/>
       <c r="D118" s="9"/>
       <c r="E118" s="9"/>
       <c r="F118" s="9"/>
-      <c r="G118" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="H118" s="17" t="s">
-        <v>114</v>
-      </c>
+      <c r="G118" s="9"/>
+      <c r="H118" s="17"/>
       <c r="I118" s="2"/>
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
@@ -6203,14 +6215,14 @@
       <c r="R119" s="2"/>
     </row>
     <row r="120" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="12"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
-      <c r="G120" s="9"/>
-      <c r="H120" s="17"/>
+      <c r="A120" s="2"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="14"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="2"/>
       <c r="I120" s="2"/>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
@@ -6226,10 +6238,10 @@
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
-      <c r="D121" s="14"/>
-      <c r="E121" s="14"/>
-      <c r="F121" s="14"/>
-      <c r="G121" s="14"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
       <c r="J121" s="2"/>
@@ -6365,11 +6377,10 @@
     <row r="128" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
-      <c r="G128" s="2"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
       <c r="J128" s="2"/>
@@ -6385,10 +6396,11 @@
     <row r="129" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
-      <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
-      <c r="F129" s="1"/>
-      <c r="G129" s="1"/>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
       <c r="J129" s="2"/>
@@ -6746,11 +6758,10 @@
     <row r="148" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="2"/>
-      <c r="F148" s="2"/>
-      <c r="G148" s="2"/>
+      <c r="D148" s="1"/>
+      <c r="E148" s="1"/>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
       <c r="H148" s="2"/>
       <c r="I148" s="2"/>
       <c r="J148" s="2"/>
@@ -6758,10 +6769,11 @@
     <row r="149" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
-      <c r="D149" s="1"/>
-      <c r="E149" s="1"/>
-      <c r="F149" s="1"/>
-      <c r="G149" s="1"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+      <c r="G149" s="2"/>
       <c r="H149" s="2"/>
       <c r="I149" s="2"/>
       <c r="J149" s="2"/>
@@ -6994,7 +7006,6 @@
       <c r="E161" s="2"/>
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
-      <c r="H161" s="2"/>
       <c r="I161" s="2"/>
       <c r="J161" s="2"/>
       <c r="K161" s="2"/>
@@ -7022,6 +7033,7 @@
       <c r="E162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
+      <c r="H162" s="2"/>
       <c r="I162" s="2"/>
       <c r="J162" s="2"/>
       <c r="K162" s="2"/>
@@ -7129,10 +7141,10 @@
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
-      <c r="D166" s="2"/>
-      <c r="E166" s="2"/>
-      <c r="F166" s="2"/>
-      <c r="G166" s="2"/>
+      <c r="D166" s="14"/>
+      <c r="E166" s="14"/>
+      <c r="F166" s="14"/>
+      <c r="G166" s="14"/>
       <c r="H166" s="2"/>
       <c r="I166" s="2"/>
       <c r="J166" s="2"/>
@@ -7184,13 +7196,6 @@
     </row>
     <row r="169" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A169" s="2"/>
-      <c r="B169" s="2"/>
-      <c r="C169" s="2"/>
-      <c r="D169" s="14"/>
-      <c r="E169" s="14"/>
-      <c r="F169" s="14"/>
-      <c r="G169" s="14"/>
-      <c r="H169" s="2"/>
       <c r="I169" s="2"/>
       <c r="J169" s="2"/>
       <c r="K169" s="2"/>
@@ -7203,7 +7208,6 @@
       <c r="R169" s="2"/>
     </row>
     <row r="170" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A170" s="2"/>
       <c r="I170" s="2"/>
       <c r="J170" s="2"/>
       <c r="K170" s="2"/>
@@ -8415,35 +8419,17 @@
       <c r="Z254" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="E90:H90"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:H45"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B38:H38"/>
+  <mergeCells count="47">
+    <mergeCell ref="B108:H108"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="E106:H106"/>
+    <mergeCell ref="B98:H98"/>
     <mergeCell ref="B76:H76"/>
+    <mergeCell ref="B99:H99"/>
     <mergeCell ref="B91:H91"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="E64:H64"/>
-    <mergeCell ref="B65:H65"/>
-    <mergeCell ref="B66:H66"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="E54:H54"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B55:H55"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="E75:H75"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="E97:H97"/>
+    <mergeCell ref="B107:H107"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="C2:E2"/>
@@ -8452,16 +8438,35 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B109:H109"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="E107:H107"/>
-    <mergeCell ref="B99:H99"/>
-    <mergeCell ref="B77:H77"/>
-    <mergeCell ref="B100:H100"/>
-    <mergeCell ref="B92:H92"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="E98:H98"/>
-    <mergeCell ref="B108:H108"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:H54"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="E74:H74"/>
+    <mergeCell ref="B75:H75"/>
+    <mergeCell ref="B90:H90"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="E63:H63"/>
+    <mergeCell ref="B64:H64"/>
+    <mergeCell ref="B65:H65"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B46:H46"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="E89:H89"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:H45"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B38:H38"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>